<commit_message>
update more experiment results of v4
</commit_message>
<xml_diff>
--- a/v4/v4_standard/v4_initial_std_regression.xlsx
+++ b/v4/v4_standard/v4_initial_std_regression.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\master\ensemble_github\v3+\analysis_data\std_missing_value\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\master\ensemble_github\experimental_data\v4\v4_standard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38E27E39-BE19-4961-9B28-BCE448D4EB74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BC3813E-365A-47B0-B7CD-8BE21D9A8E0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15" yWindow="330" windowWidth="21570" windowHeight="12570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="262">
   <si>
     <t>dataname:task_type</t>
   </si>
@@ -803,13 +803,17 @@
   </si>
   <si>
     <t>-13.68%</t>
+  </si>
+  <si>
+    <t>default setting of random init</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -842,13 +846,33 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -878,7 +902,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -886,6 +910,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1188,1358 +1216,1364 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F67"/>
+  <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="C43" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="49.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="32.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="E1" s="6" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F2" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
         <v>23</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
         <v>28</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
         <v>33</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F8" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
         <v>38</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>39</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D9" t="s">
         <v>40</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E9" t="s">
         <v>41</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F9" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
         <v>43</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>44</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" t="s">
         <v>45</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E10" t="s">
         <v>46</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F10" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
         <v>48</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>7</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E11" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F11" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
         <v>13</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>53</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E12" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F12" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
         <v>18</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>57</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E13" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F13" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
         <v>23</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>61</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E14" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F14" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
         <v>28</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>65</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E15" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F15" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
         <v>33</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
         <v>69</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E16" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F16" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" t="s">
         <v>38</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>73</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D17" t="s">
         <v>73</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E17" t="s">
         <v>74</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F17" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" t="s">
         <v>43</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>44</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D18" t="s">
         <v>76</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E18" t="s">
         <v>77</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F18" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A19" t="s">
         <v>79</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>7</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>80</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F19" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>12</v>
-      </c>
-      <c r="B19" t="s">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" t="s">
         <v>13</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
         <v>84</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D20" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F20" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" t="s">
         <v>18</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>88</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D21" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E21" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F21" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>12</v>
-      </c>
-      <c r="B21" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" t="s">
         <v>23</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" t="s">
         <v>92</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F22" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>12</v>
-      </c>
-      <c r="B22" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" t="s">
         <v>28</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" t="s">
         <v>96</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D23" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E23" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="F23" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>12</v>
-      </c>
-      <c r="B23" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" t="s">
         <v>33</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>100</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D24" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E24" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F24" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>12</v>
-      </c>
-      <c r="B24" t="s">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A25" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" t="s">
         <v>38</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>104</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D25" t="s">
         <v>39</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E25" t="s">
         <v>104</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F25" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>12</v>
-      </c>
-      <c r="B25" t="s">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A26" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" t="s">
         <v>43</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C26" t="s">
         <v>44</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D26" t="s">
         <v>105</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E26" t="s">
         <v>106</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F26" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A27" t="s">
         <v>108</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>7</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>109</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="E27" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="F27" s="3" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>12</v>
-      </c>
-      <c r="B27" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A28" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" t="s">
         <v>13</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C28" t="s">
         <v>113</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="E28" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="F28" s="3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>12</v>
-      </c>
-      <c r="B28" t="s">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A29" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" t="s">
         <v>18</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C29" t="s">
         <v>117</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D29" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="E29" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="F29" s="3" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>12</v>
-      </c>
-      <c r="B29" t="s">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A30" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" t="s">
         <v>23</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C30" t="s">
         <v>121</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D30" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="E30" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="F30" s="3" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>12</v>
-      </c>
-      <c r="B30" t="s">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A31" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31" t="s">
         <v>28</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" t="s">
         <v>125</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D31" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="E30" s="3" t="s">
+      <c r="E31" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="F31" s="3" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>12</v>
-      </c>
-      <c r="B31" t="s">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A32" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32" t="s">
         <v>33</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C32" t="s">
         <v>129</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D32" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="E32" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="F32" s="3" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>12</v>
-      </c>
-      <c r="B32" t="s">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A33" t="s">
+        <v>12</v>
+      </c>
+      <c r="B33" t="s">
         <v>38</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C33" t="s">
         <v>73</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D33" t="s">
         <v>42</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E33" t="s">
         <v>39</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F33" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>12</v>
-      </c>
-      <c r="B33" t="s">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A34" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" t="s">
         <v>43</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C34" t="s">
         <v>44</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D34" t="s">
         <v>134</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E34" t="s">
         <v>135</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F34" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A35" t="s">
         <v>137</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
         <v>7</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C35" t="s">
         <v>138</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D35" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="E34" s="3" t="s">
+      <c r="E35" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="F34" s="3" t="s">
+      <c r="F35" s="3" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>12</v>
-      </c>
-      <c r="B35" t="s">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A36" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" t="s">
         <v>13</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C36" t="s">
         <v>142</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D36" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="E35" s="3" t="s">
+      <c r="E36" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="F35" s="3" t="s">
+      <c r="F36" s="3" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>12</v>
-      </c>
-      <c r="B36" t="s">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A37" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37" t="s">
         <v>18</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C37" t="s">
         <v>146</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="D37" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E36" s="3" t="s">
+      <c r="E37" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="F36" s="3" t="s">
+      <c r="F37" s="3" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>12</v>
-      </c>
-      <c r="B37" t="s">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A38" t="s">
+        <v>12</v>
+      </c>
+      <c r="B38" t="s">
         <v>23</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C38" t="s">
         <v>150</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="D38" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="E37" s="3" t="s">
+      <c r="E38" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="F37" s="3" t="s">
+      <c r="F38" s="3" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>12</v>
-      </c>
-      <c r="B38" t="s">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A39" t="s">
+        <v>12</v>
+      </c>
+      <c r="B39" t="s">
         <v>28</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C39" t="s">
         <v>154</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="D39" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="E38" s="2" t="s">
+      <c r="E39" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="F38" s="3" t="s">
+      <c r="F39" s="3" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>12</v>
-      </c>
-      <c r="B39" t="s">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A40" t="s">
+        <v>12</v>
+      </c>
+      <c r="B40" t="s">
         <v>33</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C40" t="s">
         <v>158</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="D40" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="E39" s="3" t="s">
+      <c r="E40" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="F39" s="3" t="s">
+      <c r="F40" s="3" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>12</v>
-      </c>
-      <c r="B40" t="s">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A41" t="s">
+        <v>12</v>
+      </c>
+      <c r="B41" t="s">
         <v>38</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C41" t="s">
         <v>42</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D41" t="s">
         <v>73</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E41" t="s">
         <v>162</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F41" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>12</v>
-      </c>
-      <c r="B41" t="s">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A42" t="s">
+        <v>12</v>
+      </c>
+      <c r="B42" t="s">
         <v>43</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C42" t="s">
         <v>44</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D42" t="s">
         <v>164</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E42" t="s">
         <v>165</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F42" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A43" t="s">
         <v>167</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" t="s">
         <v>7</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C43" t="s">
         <v>168</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="D43" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="E42" s="2" t="s">
+      <c r="E43" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="F42" s="3" t="s">
+      <c r="F43" s="3" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>12</v>
-      </c>
-      <c r="B43" t="s">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A44" t="s">
+        <v>12</v>
+      </c>
+      <c r="B44" t="s">
         <v>13</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C44" t="s">
         <v>172</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="D44" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="E43" s="2" t="s">
+      <c r="E44" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="F43" s="2" t="s">
+      <c r="F44" s="2" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>12</v>
-      </c>
-      <c r="B44" t="s">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A45" t="s">
+        <v>12</v>
+      </c>
+      <c r="B45" t="s">
         <v>18</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C45" t="s">
         <v>176</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="D45" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="E44" s="3" t="s">
+      <c r="E45" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="F44" s="2" t="s">
+      <c r="F45" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>12</v>
-      </c>
-      <c r="B45" t="s">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A46" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46" t="s">
         <v>23</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C46" t="s">
         <v>180</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="D46" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="E45" s="2" t="s">
+      <c r="E46" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="F45" s="2" t="s">
+      <c r="F46" s="2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>12</v>
-      </c>
-      <c r="B46" t="s">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A47" t="s">
+        <v>12</v>
+      </c>
+      <c r="B47" t="s">
         <v>28</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C47" t="s">
         <v>184</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="D47" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="E46" s="2" t="s">
+      <c r="E47" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="F46" s="2" t="s">
+      <c r="F47" s="2" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>12</v>
-      </c>
-      <c r="B47" t="s">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A48" t="s">
+        <v>12</v>
+      </c>
+      <c r="B48" t="s">
         <v>33</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C48" t="s">
         <v>188</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="D48" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="E47" s="2" t="s">
+      <c r="E48" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="F47" s="2" t="s">
+      <c r="F48" s="2" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>12</v>
-      </c>
-      <c r="B48" t="s">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A49" t="s">
+        <v>12</v>
+      </c>
+      <c r="B49" t="s">
         <v>38</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C49" t="s">
         <v>133</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D49" t="s">
         <v>192</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E49" t="s">
         <v>193</v>
       </c>
-      <c r="F48" t="s">
+      <c r="F49" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>12</v>
-      </c>
-      <c r="B49" t="s">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A50" t="s">
+        <v>12</v>
+      </c>
+      <c r="B50" t="s">
         <v>43</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C50" t="s">
         <v>44</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D50" t="s">
         <v>194</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E50" t="s">
         <v>195</v>
       </c>
-      <c r="F49" t="s">
+      <c r="F50" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A51" t="s">
         <v>197</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B51" t="s">
         <v>7</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C51" t="s">
         <v>198</v>
       </c>
-      <c r="D50" s="2" t="s">
+      <c r="D51" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="E50" s="3" t="s">
+      <c r="E51" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="F50" s="3" t="s">
+      <c r="F51" s="3" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>12</v>
-      </c>
-      <c r="B51" t="s">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A52" t="s">
+        <v>12</v>
+      </c>
+      <c r="B52" t="s">
         <v>13</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C52" t="s">
         <v>202</v>
       </c>
-      <c r="D51" s="3" t="s">
+      <c r="D52" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="E51" s="3" t="s">
+      <c r="E52" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="F51" s="3" t="s">
+      <c r="F52" s="3" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>12</v>
-      </c>
-      <c r="B52" t="s">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A53" t="s">
+        <v>12</v>
+      </c>
+      <c r="B53" t="s">
         <v>18</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C53" t="s">
         <v>206</v>
       </c>
-      <c r="D52" s="3" t="s">
+      <c r="D53" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="E52" s="3" t="s">
+      <c r="E53" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="F52" s="3" t="s">
+      <c r="F53" s="3" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>12</v>
-      </c>
-      <c r="B53" t="s">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A54" t="s">
+        <v>12</v>
+      </c>
+      <c r="B54" t="s">
         <v>23</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C54" t="s">
         <v>210</v>
       </c>
-      <c r="D53" s="3" t="s">
+      <c r="D54" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="E53" s="3" t="s">
+      <c r="E54" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="F53" s="3" t="s">
+      <c r="F54" s="3" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>12</v>
-      </c>
-      <c r="B54" t="s">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A55" t="s">
+        <v>12</v>
+      </c>
+      <c r="B55" t="s">
         <v>28</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C55" t="s">
         <v>214</v>
       </c>
-      <c r="D54" s="3" t="s">
+      <c r="D55" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="E54" s="3" t="s">
+      <c r="E55" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="F54" s="2" t="s">
+      <c r="F55" s="2" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>12</v>
-      </c>
-      <c r="B55" t="s">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A56" t="s">
+        <v>12</v>
+      </c>
+      <c r="B56" t="s">
         <v>33</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C56" t="s">
         <v>218</v>
       </c>
-      <c r="D55" s="3" t="s">
+      <c r="D56" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="E55" s="3" t="s">
+      <c r="E56" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="F55" s="3" t="s">
+      <c r="F56" s="3" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>12</v>
-      </c>
-      <c r="B56" t="s">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A57" t="s">
+        <v>12</v>
+      </c>
+      <c r="B57" t="s">
         <v>38</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C57" t="s">
         <v>222</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D57" t="s">
         <v>74</v>
       </c>
-      <c r="E56" t="s">
+      <c r="E57" t="s">
         <v>193</v>
       </c>
-      <c r="F56" t="s">
+      <c r="F57" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>12</v>
-      </c>
-      <c r="B57" t="s">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A58" t="s">
+        <v>12</v>
+      </c>
+      <c r="B58" t="s">
         <v>43</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C58" t="s">
         <v>44</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D58" t="s">
         <v>223</v>
       </c>
-      <c r="E57" t="s">
+      <c r="E58" t="s">
         <v>224</v>
       </c>
-      <c r="F57" t="s">
+      <c r="F58" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A59" t="s">
         <v>226</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B59" t="s">
         <v>7</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C59" t="s">
         <v>227</v>
       </c>
-      <c r="D58" s="3" t="s">
+      <c r="D59" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="E58" s="3" t="s">
+      <c r="E59" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="F58" s="3" t="s">
+      <c r="F59" s="3" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>12</v>
-      </c>
-      <c r="B59" t="s">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A60" t="s">
+        <v>12</v>
+      </c>
+      <c r="B60" t="s">
         <v>13</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C60" t="s">
         <v>231</v>
       </c>
-      <c r="D59" s="3" t="s">
+      <c r="D60" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="E59" s="3" t="s">
+      <c r="E60" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="F59" s="3" t="s">
+      <c r="F60" s="3" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>12</v>
-      </c>
-      <c r="B60" t="s">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A61" t="s">
+        <v>12</v>
+      </c>
+      <c r="B61" t="s">
         <v>18</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C61" t="s">
         <v>235</v>
       </c>
-      <c r="D60" s="2" t="s">
+      <c r="D61" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="E60" s="3" t="s">
+      <c r="E61" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="F60" s="2" t="s">
+      <c r="F61" s="2" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>12</v>
-      </c>
-      <c r="B61" t="s">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A62" t="s">
+        <v>12</v>
+      </c>
+      <c r="B62" t="s">
         <v>23</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C62" t="s">
         <v>239</v>
       </c>
-      <c r="D61" s="3" t="s">
+      <c r="D62" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="E61" s="3" t="s">
+      <c r="E62" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="F61" s="3" t="s">
+      <c r="F62" s="3" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>12</v>
-      </c>
-      <c r="B62" t="s">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A63" t="s">
+        <v>12</v>
+      </c>
+      <c r="B63" t="s">
         <v>28</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C63" t="s">
         <v>243</v>
       </c>
-      <c r="D62" s="3" t="s">
+      <c r="D63" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="E62" s="3" t="s">
+      <c r="E63" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="F62" s="3" t="s">
+      <c r="F63" s="3" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>12</v>
-      </c>
-      <c r="B63" t="s">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A64" t="s">
+        <v>12</v>
+      </c>
+      <c r="B64" t="s">
         <v>33</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C64" t="s">
         <v>247</v>
       </c>
-      <c r="D63" s="3" t="s">
+      <c r="D64" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="E63" s="3" t="s">
+      <c r="E64" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="F63" s="3" t="s">
+      <c r="F64" s="3" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>12</v>
-      </c>
-      <c r="B64" t="s">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A65" t="s">
+        <v>12</v>
+      </c>
+      <c r="B65" t="s">
         <v>38</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C65" t="s">
         <v>222</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D65" t="s">
         <v>251</v>
       </c>
-      <c r="E64" t="s">
+      <c r="E65" t="s">
         <v>252</v>
       </c>
-      <c r="F64" t="s">
+      <c r="F65" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>12</v>
-      </c>
-      <c r="B65" t="s">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A66" t="s">
+        <v>12</v>
+      </c>
+      <c r="B66" t="s">
         <v>43</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C66" t="s">
         <v>44</v>
       </c>
-      <c r="D65" t="s">
+      <c r="D66" t="s">
         <v>253</v>
       </c>
-      <c r="E65" t="s">
+      <c r="E66" t="s">
         <v>254</v>
       </c>
-      <c r="F65" t="s">
+      <c r="F66" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>12</v>
-      </c>
-      <c r="B66" t="s">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A67" t="s">
+        <v>12</v>
+      </c>
+      <c r="B67" t="s">
         <v>256</v>
       </c>
-      <c r="C66" s="4">
+      <c r="C67" s="4">
         <v>2.895833333333333</v>
       </c>
-      <c r="D66" s="4">
+      <c r="D67" s="4">
         <v>2.895833333333333</v>
       </c>
-      <c r="E66" s="4">
+      <c r="E67" s="4">
         <v>2.083333333333333</v>
       </c>
-      <c r="F66" s="4">
+      <c r="F67" s="4">
         <v>2.125</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>12</v>
-      </c>
-      <c r="B67" t="s">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A68" t="s">
+        <v>12</v>
+      </c>
+      <c r="B68" t="s">
         <v>257</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C68" t="s">
         <v>44</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D68" t="s">
         <v>258</v>
       </c>
-      <c r="E67" t="s">
+      <c r="E68" t="s">
         <v>259</v>
       </c>
-      <c r="F67" t="s">
+      <c r="F68" t="s">
         <v>260</v>
       </c>
     </row>

</xml_diff>